<commit_message>
new plots on linkages and fixed plots on footprints
</commit_message>
<xml_diff>
--- a/Shocks/ShockMaster.xlsx
+++ b/Shocks/ShockMaster.xlsx
@@ -8,10 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\loren\Documents\GitHub\MARIO Organization\GreenTechs\Shocks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A3A1B49-A313-469F-9931-DF662E88467E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4D7FCE8-9A4C-4365-90C1-D78328CECECF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{7AC5AC57-1F64-4F2D-BB65-F878D395C517}"/>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" activeTab="1" xr2:uid="{FDEE0995-F68A-4ED9-9CCF-85B3630CFFD1}"/>
+    <workbookView xWindow="39852" yWindow="0" windowWidth="9396" windowHeight="13200" activeTab="1" xr2:uid="{B60DDE52-988F-44A2-B15C-F9EEC5148EBF}"/>
   </bookViews>
   <sheets>
     <sheet name="ShockMaster" sheetId="6" r:id="rId1"/>
@@ -24,7 +23,7 @@
     <sheet name="EXIOHSUT_Electricity prices" sheetId="5" r:id="rId8"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">ShockMaster!$A$1:$M$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">ShockMaster!$A$1:$M$409</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -675,15 +674,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{97D578EE-3C05-4D0C-AE17-43AAD0A9E4AC}">
-  <sheetPr>
+  <sheetPr filterMode="1">
     <tabColor theme="1"/>
   </sheetPr>
   <dimension ref="A1:M409"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A373" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H407" sqref="H407"/>
-    </sheetView>
-    <sheetView workbookViewId="1"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -743,7 +739,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>20</v>
       </c>
@@ -777,7 +773,7 @@
         <v>0.31791623705013017</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>20</v>
       </c>
@@ -811,7 +807,7 @@
         <v>8.4052867968024844E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>20</v>
       </c>
@@ -845,7 +841,7 @@
         <v>0.15997266486503273</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>20</v>
       </c>
@@ -879,7 +875,7 @@
         <v>0.31216209701302372</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>20</v>
       </c>
@@ -913,7 +909,7 @@
         <v>8.2531549090775522E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>20</v>
       </c>
@@ -947,7 +943,7 @@
         <v>0.15707723201679688</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>20</v>
       </c>
@@ -981,7 +977,7 @@
         <v>0.31216209701302372</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>20</v>
       </c>
@@ -1015,7 +1011,7 @@
         <v>8.2531549090775522E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>20</v>
       </c>
@@ -1049,7 +1045,7 @@
         <v>0.15707723201679688</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>20</v>
       </c>
@@ -1083,7 +1079,7 @@
         <v>0.31075596144089296</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>20</v>
       </c>
@@ -1117,7 +1113,7 @@
         <v>8.2159785356132387E-2</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>20</v>
       </c>
@@ -1151,7 +1147,7 @@
         <v>0.1563696769176221</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>20</v>
       </c>
@@ -1185,7 +1181,7 @@
         <v>0.31216209701302372</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>20</v>
       </c>
@@ -1219,7 +1215,7 @@
         <v>8.2531549090775522E-2</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>20</v>
       </c>
@@ -1253,7 +1249,7 @@
         <v>0.15707723201679688</v>
       </c>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>20</v>
       </c>
@@ -1287,7 +1283,7 @@
         <v>0.3135810156358102</v>
       </c>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>20</v>
       </c>
@@ -1321,7 +1317,7 @@
         <v>8.2906692495733597E-2</v>
       </c>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>20</v>
       </c>
@@ -1355,7 +1351,7 @@
         <v>0.15779121943505503</v>
       </c>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>20</v>
       </c>
@@ -1389,7 +1385,7 @@
         <v>0.31216209701302372</v>
       </c>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>20</v>
       </c>
@@ -1423,7 +1419,7 @@
         <v>8.2531549090775522E-2</v>
       </c>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>20</v>
       </c>
@@ -1457,7 +1453,7 @@
         <v>0.15707723201679688</v>
       </c>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>20</v>
       </c>
@@ -1491,7 +1487,7 @@
         <v>0.30936243695012666</v>
       </c>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>20</v>
       </c>
@@ -1525,7 +1521,7 @@
         <v>8.1791355825387407E-2</v>
       </c>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>20</v>
       </c>
@@ -1559,7 +1555,7 @@
         <v>0.15566846760409017</v>
       </c>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>20</v>
       </c>
@@ -1593,7 +1589,7 @@
         <v>0.30661254862168102</v>
       </c>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>20</v>
       </c>
@@ -1627,7 +1623,7 @@
         <v>8.1064321551383961E-2</v>
       </c>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>20</v>
       </c>
@@ -1661,7 +1657,7 @@
         <v>0.15428474789205379</v>
       </c>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>33</v>
       </c>
@@ -1695,7 +1691,7 @@
         <v>0.81472674795357813</v>
       </c>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>33</v>
       </c>
@@ -1729,7 +1725,7 @@
         <v>0.21540302694562333</v>
       </c>
     </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>33</v>
       </c>
@@ -1763,7 +1759,7 @@
         <v>0.40996336084087537</v>
       </c>
     </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>33</v>
       </c>
@@ -1797,7 +1793,7 @@
         <v>0.81312420338824976</v>
       </c>
     </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>33</v>
       </c>
@@ -1831,7 +1827,7 @@
         <v>0.21497933525874297</v>
       </c>
     </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>33</v>
       </c>
@@ -1865,7 +1861,7 @@
         <v>0.40915697445728166</v>
       </c>
     </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>33</v>
       </c>
@@ -1899,7 +1895,7 @@
         <v>0.80074082768436972</v>
       </c>
     </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>33</v>
       </c>
@@ -1933,7 +1929,7 @@
         <v>0.21170533373968076</v>
       </c>
     </row>
-    <row r="37" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>33</v>
       </c>
@@ -1967,7 +1963,7 @@
         <v>0.40292576830764987</v>
       </c>
     </row>
-    <row r="38" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>33</v>
       </c>
@@ -2001,7 +1997,7 @@
         <v>0.8120724534316448</v>
       </c>
     </row>
-    <row r="39" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>33</v>
       </c>
@@ -2035,7 +2031,7 @@
         <v>0.21470126641564719</v>
       </c>
     </row>
-    <row r="40" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>33</v>
       </c>
@@ -2069,7 +2065,7 @@
         <v>0.40862774309467198</v>
       </c>
     </row>
-    <row r="41" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>33</v>
       </c>
@@ -2103,7 +2099,7 @@
         <v>0.82478248388439546</v>
       </c>
     </row>
-    <row r="42" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>33</v>
       </c>
@@ -2137,7 +2133,7 @@
         <v>0.21806163115016741</v>
       </c>
     </row>
-    <row r="43" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>33</v>
       </c>
@@ -2171,7 +2167,7 @@
         <v>0.41502331905174916</v>
       </c>
     </row>
-    <row r="44" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>33</v>
       </c>
@@ -2205,7 +2201,7 @@
         <v>0.85616637136841112</v>
       </c>
     </row>
-    <row r="45" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>33</v>
       </c>
@@ -2239,7 +2235,7 @@
         <v>0.22635911785765309</v>
       </c>
     </row>
-    <row r="46" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>33</v>
       </c>
@@ -2273,7 +2269,7 @@
         <v>0.43081541624447817</v>
       </c>
     </row>
-    <row r="47" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>33</v>
       </c>
@@ -2307,7 +2303,7 @@
         <v>0.85044556295581764</v>
       </c>
     </row>
-    <row r="48" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>33</v>
       </c>
@@ -2341,7 +2337,7 @@
         <v>0.22484661142314133</v>
       </c>
     </row>
-    <row r="49" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>33</v>
       </c>
@@ -2375,7 +2371,7 @@
         <v>0.42793675557764166</v>
       </c>
     </row>
-    <row r="50" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>33</v>
       </c>
@@ -2409,7 +2405,7 @@
         <v>0.79603060270441095</v>
       </c>
     </row>
-    <row r="51" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>33</v>
       </c>
@@ -2443,7 +2439,7 @@
         <v>0.21046001226125075</v>
       </c>
     </row>
-    <row r="52" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>33</v>
       </c>
@@ -2477,7 +2473,7 @@
         <v>0.40055562436926695</v>
       </c>
     </row>
-    <row r="53" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>33</v>
       </c>
@@ -2511,7 +2507,7 @@
         <v>0.77302799559110935</v>
       </c>
     </row>
-    <row r="54" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>33</v>
       </c>
@@ -2545,7 +2541,7 @@
         <v>0.20437842575105997</v>
       </c>
     </row>
-    <row r="55" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>33</v>
       </c>
@@ -2579,7 +2575,7 @@
         <v>0.38898091402133972</v>
       </c>
     </row>
-    <row r="56" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>34</v>
       </c>
@@ -2613,7 +2609,7 @@
         <v>0.79250778065167293</v>
       </c>
     </row>
-    <row r="57" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>34</v>
       </c>
@@ -2647,7 +2643,7 @@
         <v>0.20952862448558662</v>
       </c>
     </row>
-    <row r="58" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>34</v>
       </c>
@@ -2681,7 +2677,7 @@
         <v>0.39878297117970074</v>
       </c>
     </row>
-    <row r="59" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>34</v>
       </c>
@@ -2715,7 +2711,7 @@
         <v>0.79250778065167293</v>
       </c>
     </row>
-    <row r="60" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>34</v>
       </c>
@@ -2749,7 +2745,7 @@
         <v>0.20952862448558662</v>
       </c>
     </row>
-    <row r="61" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>34</v>
       </c>
@@ -2783,7 +2779,7 @@
         <v>0.39878297117970074</v>
       </c>
     </row>
-    <row r="62" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>34</v>
       </c>
@@ -2817,7 +2813,7 @@
         <v>0.79250778065167293</v>
       </c>
     </row>
-    <row r="63" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>34</v>
       </c>
@@ -2851,7 +2847,7 @@
         <v>0.20952862448558662</v>
       </c>
     </row>
-    <row r="64" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>34</v>
       </c>
@@ -2885,7 +2881,7 @@
         <v>0.39878297117970074</v>
       </c>
     </row>
-    <row r="65" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>34</v>
       </c>
@@ -2919,7 +2915,7 @@
         <v>0.79250778065167293</v>
       </c>
     </row>
-    <row r="66" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>34</v>
       </c>
@@ -2953,7 +2949,7 @@
         <v>0.20952862448558662</v>
       </c>
     </row>
-    <row r="67" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>34</v>
       </c>
@@ -2987,7 +2983,7 @@
         <v>0.39878297117970074</v>
       </c>
     </row>
-    <row r="68" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>34</v>
       </c>
@@ -3021,7 +3017,7 @@
         <v>0.79250778065167293</v>
       </c>
     </row>
-    <row r="69" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>34</v>
       </c>
@@ -3055,7 +3051,7 @@
         <v>0.20952862448558662</v>
       </c>
     </row>
-    <row r="70" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>34</v>
       </c>
@@ -3089,7 +3085,7 @@
         <v>0.39878297117970074</v>
       </c>
     </row>
-    <row r="71" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>34</v>
       </c>
@@ -3123,7 +3119,7 @@
         <v>0.79250778065167293</v>
       </c>
     </row>
-    <row r="72" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>34</v>
       </c>
@@ -3157,7 +3153,7 @@
         <v>0.20952862448558662</v>
       </c>
     </row>
-    <row r="73" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>34</v>
       </c>
@@ -3191,7 +3187,7 @@
         <v>0.39878297117970074</v>
       </c>
     </row>
-    <row r="74" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>34</v>
       </c>
@@ -3225,7 +3221,7 @@
         <v>0.79250778065167293</v>
       </c>
     </row>
-    <row r="75" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>34</v>
       </c>
@@ -3259,7 +3255,7 @@
         <v>0.20952862448558662</v>
       </c>
     </row>
-    <row r="76" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>34</v>
       </c>
@@ -3293,7 +3289,7 @@
         <v>0.39878297117970074</v>
       </c>
     </row>
-    <row r="77" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>34</v>
       </c>
@@ -3327,7 +3323,7 @@
         <v>0.79250778065167293</v>
       </c>
     </row>
-    <row r="78" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>34</v>
       </c>
@@ -3361,7 +3357,7 @@
         <v>0.20952862448558662</v>
       </c>
     </row>
-    <row r="79" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>34</v>
       </c>
@@ -3395,7 +3391,7 @@
         <v>0.39878297117970074</v>
       </c>
     </row>
-    <row r="80" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>34</v>
       </c>
@@ -3429,7 +3425,7 @@
         <v>0.79250778065167293</v>
       </c>
     </row>
-    <row r="81" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>34</v>
       </c>
@@ -3463,7 +3459,7 @@
         <v>0.20952862448558662</v>
       </c>
     </row>
-    <row r="82" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>34</v>
       </c>
@@ -3497,7 +3493,7 @@
         <v>0.39878297117970074</v>
       </c>
     </row>
-    <row r="83" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>20</v>
       </c>
@@ -3531,7 +3527,7 @@
         <v>0.2384371777875976</v>
       </c>
     </row>
-    <row r="84" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>20</v>
       </c>
@@ -3565,7 +3561,7 @@
         <v>5.4033986550873103E-2</v>
       </c>
     </row>
-    <row r="85" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>20</v>
       </c>
@@ -3599,7 +3595,7 @@
         <v>0.10498206131767777</v>
       </c>
     </row>
-    <row r="86" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>20</v>
       </c>
@@ -3633,7 +3629,7 @@
         <v>0.23412157275976775</v>
       </c>
     </row>
-    <row r="87" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>20</v>
       </c>
@@ -3667,7 +3663,7 @@
         <v>5.3055995844069968E-2</v>
       </c>
     </row>
-    <row r="88" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>20</v>
       </c>
@@ -3701,7 +3697,7 @@
         <v>0.10308193351102297</v>
       </c>
     </row>
-    <row r="89" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>20</v>
       </c>
@@ -3735,7 +3731,7 @@
         <v>0.23412157275976775</v>
       </c>
     </row>
-    <row r="90" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>20</v>
       </c>
@@ -3769,7 +3765,7 @@
         <v>5.3055995844069968E-2</v>
       </c>
     </row>
-    <row r="91" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>20</v>
       </c>
@@ -3803,7 +3799,7 @@
         <v>0.10308193351102297</v>
       </c>
     </row>
-    <row r="92" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>20</v>
       </c>
@@ -3837,7 +3833,7 @@
         <v>0.2330669710806697</v>
       </c>
     </row>
-    <row r="93" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>20</v>
       </c>
@@ -3871,7 +3867,7 @@
         <v>5.281700487179939E-2</v>
       </c>
     </row>
-    <row r="94" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>20</v>
       </c>
@@ -3905,7 +3901,7 @@
         <v>0.10261760047718953</v>
       </c>
     </row>
-    <row r="95" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>20</v>
       </c>
@@ -3939,7 +3935,7 @@
         <v>0.23412157275976775</v>
       </c>
     </row>
-    <row r="96" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>20</v>
       </c>
@@ -3973,7 +3969,7 @@
         <v>5.3055995844069968E-2</v>
       </c>
     </row>
-    <row r="97" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>20</v>
       </c>
@@ -4007,7 +4003,7 @@
         <v>0.10308193351102297</v>
       </c>
     </row>
-    <row r="98" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>20</v>
       </c>
@@ -4041,7 +4037,7 @@
         <v>0.23518576172685762</v>
       </c>
     </row>
-    <row r="99" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>20</v>
       </c>
@@ -4075,7 +4071,7 @@
         <v>5.3297159461543016E-2</v>
       </c>
     </row>
-    <row r="100" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>20</v>
       </c>
@@ -4109,7 +4105,7 @@
         <v>0.10355048775425489</v>
       </c>
     </row>
-    <row r="101" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>20</v>
       </c>
@@ -4143,7 +4139,7 @@
         <v>0.23412157275976775</v>
       </c>
     </row>
-    <row r="102" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>20</v>
       </c>
@@ -4177,7 +4173,7 @@
         <v>5.3055995844069968E-2</v>
       </c>
     </row>
-    <row r="103" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
         <v>20</v>
       </c>
@@ -4211,7 +4207,7 @@
         <v>0.10308193351102297</v>
       </c>
     </row>
-    <row r="104" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
         <v>20</v>
       </c>
@@ -4245,7 +4241,7 @@
         <v>0.23202182771259494</v>
       </c>
     </row>
-    <row r="105" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
         <v>20</v>
       </c>
@@ -4279,7 +4275,7 @@
         <v>5.2580157316320465E-2</v>
       </c>
     </row>
-    <row r="106" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
         <v>20</v>
       </c>
@@ -4313,7 +4309,7 @@
         <v>0.1021574318651842</v>
       </c>
     </row>
-    <row r="107" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
         <v>20</v>
       </c>
@@ -4347,7 +4343,7 @@
         <v>0.22995941146626075</v>
       </c>
     </row>
-    <row r="108" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
         <v>20</v>
       </c>
@@ -4381,7 +4377,7 @@
         <v>5.2112778140175398E-2</v>
       </c>
     </row>
-    <row r="109" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
         <v>20</v>
       </c>
@@ -4415,7 +4411,7 @@
         <v>0.10124936580416033</v>
       </c>
     </row>
-    <row r="110" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
         <v>33</v>
       </c>
@@ -4449,7 +4445,7 @@
         <v>0.61104506096518352</v>
       </c>
     </row>
-    <row r="111" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
         <v>33</v>
       </c>
@@ -4483,7 +4479,7 @@
         <v>0.13847337446504354</v>
       </c>
     </row>
-    <row r="112" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
         <v>33</v>
       </c>
@@ -4517,7 +4513,7 @@
         <v>0.26903845555182448</v>
       </c>
     </row>
-    <row r="113" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
         <v>33</v>
       </c>
@@ -4551,7 +4547,7 @@
         <v>0.60984315254118726</v>
       </c>
     </row>
-    <row r="114" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
         <v>33</v>
       </c>
@@ -4585,7 +4581,7 @@
         <v>0.13820100123776333</v>
       </c>
     </row>
-    <row r="115" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
         <v>33</v>
       </c>
@@ -4619,7 +4615,7 @@
         <v>0.26850926448759116</v>
       </c>
     </row>
-    <row r="116" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
         <v>33</v>
       </c>
@@ -4653,7 +4649,7 @@
         <v>0.60055562076327729</v>
       </c>
     </row>
-    <row r="117" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
         <v>33</v>
       </c>
@@ -4687,7 +4683,7 @@
         <v>0.13609628597550902</v>
       </c>
     </row>
-    <row r="118" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
         <v>33</v>
       </c>
@@ -4721,7 +4717,7 @@
         <v>0.26442003545189524</v>
       </c>
     </row>
-    <row r="119" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
         <v>33</v>
       </c>
@@ -4755,7 +4751,7 @@
         <v>0.60905434007373349</v>
       </c>
     </row>
-    <row r="120" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
         <v>33</v>
       </c>
@@ -4789,7 +4785,7 @@
         <v>0.13802224269577318</v>
       </c>
     </row>
-    <row r="121" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
         <v>33</v>
       </c>
@@ -4823,7 +4819,7 @@
         <v>0.26816195640587859</v>
       </c>
     </row>
-    <row r="122" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
         <v>33</v>
       </c>
@@ -4857,7 +4853,7 @@
         <v>0.61858686291329656</v>
       </c>
     </row>
-    <row r="123" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
         <v>33</v>
       </c>
@@ -4891,7 +4887,7 @@
         <v>0.14018247716796478</v>
       </c>
     </row>
-    <row r="124" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
         <v>33</v>
       </c>
@@ -4925,7 +4921,7 @@
         <v>0.27235905312771042</v>
       </c>
     </row>
-    <row r="125" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
         <v>33</v>
       </c>
@@ -4959,7 +4955,7 @@
         <v>0.64212477852630823</v>
       </c>
     </row>
-    <row r="126" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
         <v>33</v>
       </c>
@@ -4993,7 +4989,7 @@
         <v>0.14551657576563409</v>
       </c>
     </row>
-    <row r="127" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
         <v>33</v>
       </c>
@@ -5027,7 +5023,7 @@
         <v>0.28272261691043887</v>
       </c>
     </row>
-    <row r="128" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
         <v>33</v>
       </c>
@@ -5061,7 +5057,7 @@
         <v>0.63783417221686312</v>
       </c>
     </row>
-    <row r="129" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
         <v>33</v>
       </c>
@@ -5095,7 +5091,7 @@
         <v>0.14454425020059083</v>
       </c>
     </row>
-    <row r="130" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
         <v>33</v>
       </c>
@@ -5129,7 +5125,7 @@
         <v>0.28083349584782741</v>
       </c>
     </row>
-    <row r="131" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
         <v>33</v>
       </c>
@@ -5163,7 +5159,7 @@
         <v>0.59702295202830813</v>
       </c>
     </row>
-    <row r="132" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
         <v>33</v>
       </c>
@@ -5197,7 +5193,7 @@
         <v>0.13529572216794691</v>
       </c>
     </row>
-    <row r="133" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
         <v>33</v>
       </c>
@@ -5333,7 +5329,7 @@
         <v>0.25526872482650426</v>
       </c>
     </row>
-    <row r="137" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
         <v>34</v>
       </c>
@@ -5367,7 +5363,7 @@
         <v>0.59438083548875464</v>
       </c>
     </row>
-    <row r="138" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
         <v>34</v>
       </c>
@@ -5401,7 +5397,7 @@
         <v>0.13469697288359136</v>
       </c>
     </row>
-    <row r="139" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
         <v>34</v>
       </c>
@@ -5435,7 +5431,7 @@
         <v>0.26170132483667874</v>
       </c>
     </row>
-    <row r="140" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
         <v>34</v>
       </c>
@@ -5469,7 +5465,7 @@
         <v>0.59438083548875464</v>
       </c>
     </row>
-    <row r="141" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
         <v>34</v>
       </c>
@@ -5503,7 +5499,7 @@
         <v>0.13469697288359136</v>
       </c>
     </row>
-    <row r="142" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
         <v>34</v>
       </c>
@@ -5537,7 +5533,7 @@
         <v>0.26170132483667874</v>
       </c>
     </row>
-    <row r="143" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
         <v>34</v>
       </c>
@@ -5571,7 +5567,7 @@
         <v>0.59438083548875464</v>
       </c>
     </row>
-    <row r="144" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
         <v>34</v>
       </c>
@@ -5605,7 +5601,7 @@
         <v>0.13469697288359136</v>
       </c>
     </row>
-    <row r="145" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
         <v>34</v>
       </c>
@@ -5639,7 +5635,7 @@
         <v>0.26170132483667874</v>
       </c>
     </row>
-    <row r="146" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
         <v>34</v>
       </c>
@@ -5673,7 +5669,7 @@
         <v>0.59438083548875464</v>
       </c>
     </row>
-    <row r="147" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
         <v>34</v>
       </c>
@@ -5707,7 +5703,7 @@
         <v>0.13469697288359136</v>
       </c>
     </row>
-    <row r="148" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
         <v>34</v>
       </c>
@@ -5741,7 +5737,7 @@
         <v>0.26170132483667874</v>
       </c>
     </row>
-    <row r="149" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
         <v>34</v>
       </c>
@@ -5775,7 +5771,7 @@
         <v>0.59438083548875464</v>
       </c>
     </row>
-    <row r="150" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
         <v>34</v>
       </c>
@@ -5809,7 +5805,7 @@
         <v>0.13469697288359136</v>
       </c>
     </row>
-    <row r="151" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
         <v>34</v>
       </c>
@@ -5843,7 +5839,7 @@
         <v>0.26170132483667874</v>
       </c>
     </row>
-    <row r="152" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
         <v>34</v>
       </c>
@@ -5877,7 +5873,7 @@
         <v>0.59438083548875464</v>
       </c>
     </row>
-    <row r="153" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
         <v>34</v>
       </c>
@@ -5911,7 +5907,7 @@
         <v>0.13469697288359136</v>
       </c>
     </row>
-    <row r="154" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
         <v>34</v>
       </c>
@@ -5945,7 +5941,7 @@
         <v>0.26170132483667874</v>
       </c>
     </row>
-    <row r="155" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
         <v>34</v>
       </c>
@@ -5979,7 +5975,7 @@
         <v>0.59438083548875464</v>
       </c>
     </row>
-    <row r="156" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
         <v>34</v>
       </c>
@@ -6013,7 +6009,7 @@
         <v>0.13469697288359136</v>
       </c>
     </row>
-    <row r="157" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
         <v>34</v>
       </c>
@@ -6047,7 +6043,7 @@
         <v>0.26170132483667874</v>
       </c>
     </row>
-    <row r="158" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
         <v>34</v>
       </c>
@@ -6081,7 +6077,7 @@
         <v>0.59438083548875464</v>
       </c>
     </row>
-    <row r="159" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
         <v>34</v>
       </c>
@@ -6115,7 +6111,7 @@
         <v>0.13469697288359136</v>
       </c>
     </row>
-    <row r="160" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
         <v>34</v>
       </c>
@@ -6149,7 +6145,7 @@
         <v>0.26170132483667874</v>
       </c>
     </row>
-    <row r="161" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
         <v>34</v>
       </c>
@@ -6183,7 +6179,7 @@
         <v>0.59438083548875464</v>
       </c>
     </row>
-    <row r="162" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
         <v>34</v>
       </c>
@@ -6217,7 +6213,7 @@
         <v>0.13469697288359136</v>
       </c>
     </row>
-    <row r="163" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
         <v>34</v>
       </c>
@@ -6251,7 +6247,7 @@
         <v>0.26170132483667874</v>
       </c>
     </row>
-    <row r="164" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
         <v>20</v>
       </c>
@@ -6285,7 +6281,7 @@
         <v>0.18700955120595888</v>
       </c>
     </row>
-    <row r="165" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
         <v>20</v>
       </c>
@@ -6319,7 +6315,7 @@
         <v>3.7823790585611174E-2</v>
       </c>
     </row>
-    <row r="166" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
         <v>20</v>
       </c>
@@ -6353,7 +6349,7 @@
         <v>7.4653910270348622E-2</v>
       </c>
     </row>
-    <row r="167" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
         <v>20</v>
       </c>
@@ -6387,7 +6383,7 @@
         <v>0.18362476294883745</v>
       </c>
     </row>
-    <row r="168" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
         <v>20</v>
       </c>
@@ -6421,7 +6417,7 @@
         <v>3.713919709084898E-2</v>
       </c>
     </row>
-    <row r="169" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
         <v>20</v>
       </c>
@@ -6455,7 +6451,7 @@
         <v>7.3302708274505204E-2</v>
       </c>
     </row>
-    <row r="170" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A170" t="s">
         <v>20</v>
       </c>
@@ -6489,7 +6485,7 @@
         <v>0.18362476294883745</v>
       </c>
     </row>
-    <row r="171" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
         <v>20</v>
       </c>
@@ -6523,7 +6519,7 @@
         <v>3.713919709084898E-2</v>
       </c>
     </row>
-    <row r="172" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
         <v>20</v>
       </c>
@@ -6557,7 +6553,7 @@
         <v>7.3302708274505204E-2</v>
       </c>
     </row>
-    <row r="173" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
         <v>20</v>
       </c>
@@ -6591,7 +6587,7 @@
         <v>0.18279762437699584</v>
       </c>
     </row>
-    <row r="174" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A174" t="s">
         <v>20</v>
       </c>
@@ -6625,7 +6621,7 @@
         <v>3.697190341025957E-2</v>
       </c>
     </row>
-    <row r="175" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A175" t="s">
         <v>20</v>
       </c>
@@ -6659,7 +6655,7 @@
         <v>7.297251589489033E-2</v>
       </c>
     </row>
-    <row r="176" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A176" t="s">
         <v>20</v>
       </c>
@@ -6693,7 +6689,7 @@
         <v>0.18362476294883745</v>
       </c>
     </row>
-    <row r="177" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A177" t="s">
         <v>20</v>
       </c>
@@ -6727,7 +6723,7 @@
         <v>3.713919709084898E-2</v>
       </c>
     </row>
-    <row r="178" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A178" t="s">
         <v>20</v>
       </c>
@@ -6761,7 +6757,7 @@
         <v>7.3302708274505204E-2</v>
       </c>
     </row>
-    <row r="179" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A179" t="s">
         <v>20</v>
       </c>
@@ -6795,7 +6791,7 @@
         <v>0.18445942096224124</v>
       </c>
     </row>
-    <row r="180" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A180" t="s">
         <v>20</v>
       </c>
@@ -6829,7 +6825,7 @@
         <v>3.7308011623080117E-2</v>
       </c>
     </row>
-    <row r="181" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A181" t="s">
         <v>20</v>
       </c>
@@ -6863,7 +6859,7 @@
         <v>7.3635902403025685E-2</v>
       </c>
     </row>
-    <row r="182" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A182" t="s">
         <v>20</v>
       </c>
@@ -6897,7 +6893,7 @@
         <v>0.18362476294883745</v>
       </c>
     </row>
-    <row r="183" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A183" t="s">
         <v>20</v>
       </c>
@@ -6931,7 +6927,7 @@
         <v>3.713919709084898E-2</v>
       </c>
     </row>
-    <row r="184" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A184" t="s">
         <v>20</v>
       </c>
@@ -6965,7 +6961,7 @@
         <v>7.3302708274505204E-2</v>
       </c>
     </row>
-    <row r="185" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A185" t="s">
         <v>20</v>
       </c>
@@ -6999,7 +6995,7 @@
         <v>0.18197790408830977</v>
       </c>
     </row>
-    <row r="186" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A186" t="s">
         <v>20</v>
       </c>
@@ -7033,7 +7029,7 @@
         <v>3.6806110121424325E-2</v>
       </c>
     </row>
-    <row r="187" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A187" t="s">
         <v>20</v>
       </c>
@@ -7067,7 +7063,7 @@
         <v>7.2645284881908745E-2</v>
       </c>
     </row>
-    <row r="188" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A188" t="s">
         <v>20</v>
       </c>
@@ -7101,7 +7097,7 @@
         <v>0.18036032271863589</v>
       </c>
     </row>
-    <row r="189" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A189" t="s">
         <v>20</v>
       </c>
@@ -7135,7 +7131,7 @@
         <v>3.6478944698122774E-2</v>
       </c>
     </row>
-    <row r="190" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A190" t="s">
         <v>20</v>
       </c>
@@ -7169,7 +7165,7 @@
         <v>7.1999549016291783E-2</v>
       </c>
     </row>
-    <row r="191" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A191" t="s">
         <v>33</v>
       </c>
@@ -7203,7 +7199,7 @@
         <v>0.47925102820798704</v>
       </c>
     </row>
-    <row r="192" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A192" t="s">
         <v>33</v>
       </c>
@@ -7237,7 +7233,7 @@
         <v>9.6931362125530482E-2</v>
       </c>
     </row>
-    <row r="193" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A193" t="s">
         <v>33</v>
       </c>
@@ -7271,7 +7267,7 @@
         <v>0.19131623505907516</v>
       </c>
     </row>
-    <row r="194" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A194" t="s">
         <v>33</v>
       </c>
@@ -7305,7 +7301,7 @@
         <v>0.47830835493426449</v>
       </c>
     </row>
-    <row r="195" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A195" t="s">
         <v>33</v>
       </c>
@@ -7339,7 +7335,7 @@
         <v>9.6740700866434326E-2</v>
       </c>
     </row>
-    <row r="196" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A196" t="s">
         <v>33</v>
       </c>
@@ -7373,7 +7369,7 @@
         <v>0.19093992141339813</v>
       </c>
     </row>
-    <row r="197" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A197" t="s">
         <v>33</v>
       </c>
@@ -7407,7 +7403,7 @@
         <v>0.4710240162849233</v>
       </c>
     </row>
-    <row r="198" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A198" t="s">
         <v>33</v>
       </c>
@@ -7441,7 +7437,7 @@
         <v>9.5267400182856316E-2</v>
       </c>
     </row>
-    <row r="199" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A199" t="s">
         <v>33</v>
       </c>
@@ -7475,7 +7471,7 @@
         <v>0.1880320252102366</v>
       </c>
     </row>
-    <row r="200" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A200" t="s">
         <v>33</v>
       </c>
@@ -7509,7 +7505,7 @@
         <v>0.47768967848920274</v>
       </c>
     </row>
-    <row r="201" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A201" t="s">
         <v>33</v>
       </c>
@@ -7543,7 +7539,7 @@
         <v>9.6615569887041217E-2</v>
       </c>
     </row>
-    <row r="202" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A202" t="s">
         <v>33</v>
       </c>
@@ -7577,7 +7573,7 @@
         <v>0.19069294677751361</v>
       </c>
     </row>
-    <row r="203" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A203" t="s">
         <v>33</v>
       </c>
@@ -7611,7 +7607,7 @@
         <v>0.48516616699082082</v>
       </c>
     </row>
-    <row r="204" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A204" t="s">
         <v>33</v>
       </c>
@@ -7645,7 +7641,7 @@
         <v>9.8127734017575324E-2</v>
       </c>
     </row>
-    <row r="205" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A205" t="s">
         <v>33</v>
       </c>
@@ -7679,7 +7675,7 @@
         <v>0.19367754889081629</v>
       </c>
     </row>
-    <row r="206" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A206" t="s">
         <v>33</v>
       </c>
@@ -7713,7 +7709,7 @@
         <v>0.50362727727553591</v>
       </c>
     </row>
-    <row r="207" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A207" t="s">
         <v>33</v>
       </c>
@@ -7747,7 +7743,7 @@
         <v>0.10186160303594387</v>
       </c>
     </row>
-    <row r="208" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A208" t="s">
         <v>33</v>
       </c>
@@ -7781,7 +7777,7 @@
         <v>0.20104719424742315</v>
       </c>
     </row>
-    <row r="209" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A209" t="s">
         <v>33</v>
       </c>
@@ -7815,7 +7811,7 @@
         <v>0.50026209585636328</v>
       </c>
     </row>
-    <row r="210" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A210" t="s">
         <v>33</v>
       </c>
@@ -7849,7 +7845,7 @@
         <v>0.10118097514041359</v>
       </c>
     </row>
-    <row r="211" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A211" t="s">
         <v>33</v>
       </c>
@@ -7883,7 +7879,7 @@
         <v>0.19970381926956612</v>
       </c>
     </row>
-    <row r="212" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A212" t="s">
         <v>33</v>
       </c>
@@ -7917,7 +7913,7 @@
         <v>0.46825329570847696</v>
       </c>
     </row>
-    <row r="213" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A213" t="s">
         <v>33</v>
       </c>
@@ -7951,7 +7947,7 @@
         <v>9.4707005517562823E-2</v>
       </c>
     </row>
-    <row r="214" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A214" t="s">
         <v>33</v>
       </c>
@@ -7985,7 +7981,7 @@
         <v>0.18692595803899129</v>
       </c>
     </row>
-    <row r="215" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A215" t="s">
         <v>33</v>
       </c>
@@ -8019,7 +8015,7 @@
         <v>0.4547223503477113</v>
       </c>
     </row>
-    <row r="216" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A216" t="s">
         <v>33</v>
       </c>
@@ -8053,7 +8049,7 @@
         <v>9.1970291587976968E-2</v>
       </c>
     </row>
-    <row r="217" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A217" t="s">
         <v>33</v>
       </c>
@@ -8087,7 +8083,7 @@
         <v>0.1815244265432919</v>
       </c>
     </row>
-    <row r="218" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A218" t="s">
         <v>34</v>
       </c>
@@ -8121,7 +8117,7 @@
         <v>0.46618104744216043</v>
       </c>
     </row>
-    <row r="219" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A219" t="s">
         <v>34</v>
       </c>
@@ -8155,7 +8151,7 @@
         <v>9.4287881018513972E-2</v>
       </c>
     </row>
-    <row r="220" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A220" t="s">
         <v>34</v>
       </c>
@@ -8189,7 +8185,7 @@
         <v>0.18609871988386037</v>
       </c>
     </row>
-    <row r="221" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A221" t="s">
         <v>34</v>
       </c>
@@ -8223,7 +8219,7 @@
         <v>0.46618104744216043</v>
       </c>
     </row>
-    <row r="222" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A222" t="s">
         <v>34</v>
       </c>
@@ -8257,7 +8253,7 @@
         <v>9.4287881018513972E-2</v>
       </c>
     </row>
-    <row r="223" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A223" t="s">
         <v>34</v>
       </c>
@@ -8291,7 +8287,7 @@
         <v>0.18609871988386037</v>
       </c>
     </row>
-    <row r="224" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A224" t="s">
         <v>34</v>
       </c>
@@ -8325,7 +8321,7 @@
         <v>0.46618104744216043</v>
       </c>
     </row>
-    <row r="225" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A225" t="s">
         <v>34</v>
       </c>
@@ -8359,7 +8355,7 @@
         <v>9.4287881018513972E-2</v>
       </c>
     </row>
-    <row r="226" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A226" t="s">
         <v>34</v>
       </c>
@@ -8393,7 +8389,7 @@
         <v>0.18609871988386037</v>
       </c>
     </row>
-    <row r="227" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A227" t="s">
         <v>34</v>
       </c>
@@ -8427,7 +8423,7 @@
         <v>0.46618104744216043</v>
       </c>
     </row>
-    <row r="228" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A228" t="s">
         <v>34</v>
       </c>
@@ -8461,7 +8457,7 @@
         <v>9.4287881018513972E-2</v>
       </c>
     </row>
-    <row r="229" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="229" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A229" t="s">
         <v>34</v>
       </c>
@@ -8495,7 +8491,7 @@
         <v>0.18609871988386037</v>
       </c>
     </row>
-    <row r="230" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="230" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A230" t="s">
         <v>34</v>
       </c>
@@ -8529,7 +8525,7 @@
         <v>0.46618104744216043</v>
       </c>
     </row>
-    <row r="231" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="231" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A231" t="s">
         <v>34</v>
       </c>
@@ -8563,7 +8559,7 @@
         <v>9.4287881018513972E-2</v>
       </c>
     </row>
-    <row r="232" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="232" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A232" t="s">
         <v>34</v>
       </c>
@@ -8597,7 +8593,7 @@
         <v>0.18609871988386037</v>
       </c>
     </row>
-    <row r="233" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="233" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A233" t="s">
         <v>34</v>
       </c>
@@ -8631,7 +8627,7 @@
         <v>0.46618104744216043</v>
       </c>
     </row>
-    <row r="234" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="234" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A234" t="s">
         <v>34</v>
       </c>
@@ -8665,7 +8661,7 @@
         <v>9.4287881018513972E-2</v>
       </c>
     </row>
-    <row r="235" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="235" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A235" t="s">
         <v>34</v>
       </c>
@@ -8699,7 +8695,7 @@
         <v>0.18609871988386037</v>
       </c>
     </row>
-    <row r="236" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="236" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A236" t="s">
         <v>34</v>
       </c>
@@ -8733,7 +8729,7 @@
         <v>0.46618104744216043</v>
       </c>
     </row>
-    <row r="237" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="237" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A237" t="s">
         <v>34</v>
       </c>
@@ -8767,7 +8763,7 @@
         <v>9.4287881018513972E-2</v>
       </c>
     </row>
-    <row r="238" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="238" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A238" t="s">
         <v>34</v>
       </c>
@@ -8801,7 +8797,7 @@
         <v>0.18609871988386037</v>
       </c>
     </row>
-    <row r="239" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="239" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A239" t="s">
         <v>34</v>
       </c>
@@ -8835,7 +8831,7 @@
         <v>0.46618104744216043</v>
       </c>
     </row>
-    <row r="240" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="240" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A240" t="s">
         <v>34</v>
       </c>
@@ -8869,7 +8865,7 @@
         <v>9.4287881018513972E-2</v>
       </c>
     </row>
-    <row r="241" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="241" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A241" t="s">
         <v>34</v>
       </c>
@@ -8903,7 +8899,7 @@
         <v>0.18609871988386037</v>
       </c>
     </row>
-    <row r="242" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="242" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A242" t="s">
         <v>34</v>
       </c>
@@ -8937,7 +8933,7 @@
         <v>0.46618104744216043</v>
       </c>
     </row>
-    <row r="243" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="243" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A243" t="s">
         <v>34</v>
       </c>
@@ -8971,7 +8967,7 @@
         <v>9.4287881018513972E-2</v>
       </c>
     </row>
-    <row r="244" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="244" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A244" t="s">
         <v>34</v>
       </c>
@@ -9005,7 +9001,7 @@
         <v>0.18609871988386037</v>
       </c>
     </row>
-    <row r="245" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="245" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A245" t="s">
         <v>20</v>
       </c>
@@ -9036,7 +9032,7 @@
         <v>0.15264576294986981</v>
       </c>
     </row>
-    <row r="246" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="246" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A246" t="s">
         <v>20</v>
       </c>
@@ -9067,7 +9063,7 @@
         <v>0.20886346716694243</v>
       </c>
     </row>
-    <row r="247" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="247" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A247" t="s">
         <v>20</v>
       </c>
@@ -9098,7 +9094,7 @@
         <v>0.15839990298697626</v>
       </c>
     </row>
-    <row r="248" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="248" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A248" t="s">
         <v>20</v>
       </c>
@@ -9129,7 +9125,7 @@
         <v>0.2132802188924276</v>
       </c>
     </row>
-    <row r="249" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="249" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A249" t="s">
         <v>20</v>
       </c>
@@ -9160,7 +9156,7 @@
         <v>0.15839990298697626</v>
       </c>
     </row>
-    <row r="250" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="250" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A250" t="s">
         <v>20</v>
       </c>
@@ -9191,7 +9187,7 @@
         <v>0.2132802188924276</v>
       </c>
     </row>
-    <row r="251" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="251" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A251" t="s">
         <v>20</v>
       </c>
@@ -9222,7 +9218,7 @@
         <v>0.15980603855910702</v>
       </c>
     </row>
-    <row r="252" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="252" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A252" t="s">
         <v>20</v>
       </c>
@@ -9253,7 +9249,7 @@
         <v>0.2143595377262455</v>
       </c>
     </row>
-    <row r="253" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="253" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A253" t="s">
         <v>20</v>
       </c>
@@ -9284,7 +9280,7 @@
         <v>0.15839990298697626</v>
       </c>
     </row>
-    <row r="254" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="254" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A254" t="s">
         <v>20</v>
       </c>
@@ -9315,7 +9311,7 @@
         <v>0.2132802188924276</v>
       </c>
     </row>
-    <row r="255" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="255" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A255" t="s">
         <v>20</v>
       </c>
@@ -9346,7 +9342,7 @@
         <v>0.15698098436418978</v>
       </c>
     </row>
-    <row r="256" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="256" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A256" t="s">
         <v>20</v>
       </c>
@@ -9377,7 +9373,7 @@
         <v>0.21219108806921136</v>
       </c>
     </row>
-    <row r="257" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="257" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A257" t="s">
         <v>20</v>
       </c>
@@ -9408,7 +9404,7 @@
         <v>0.15839990298697626</v>
       </c>
     </row>
-    <row r="258" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="258" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A258" t="s">
         <v>20</v>
       </c>
@@ -9439,7 +9435,7 @@
         <v>0.2132802188924276</v>
       </c>
     </row>
-    <row r="259" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="259" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A259" t="s">
         <v>20</v>
       </c>
@@ -9470,7 +9466,7 @@
         <v>0.16119956304987332</v>
       </c>
     </row>
-    <row r="260" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="260" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A260" t="s">
         <v>20</v>
       </c>
@@ -9501,7 +9497,7 @@
         <v>0.21542917657052241</v>
       </c>
     </row>
-    <row r="261" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="261" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A261" t="s">
         <v>20</v>
       </c>
@@ -9532,7 +9528,7 @@
         <v>0.16394945137831896</v>
       </c>
     </row>
-    <row r="262" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="262" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A262" t="s">
         <v>20</v>
       </c>
@@ -9563,7 +9559,7 @@
         <v>0.21753993055656223</v>
       </c>
     </row>
-    <row r="263" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="263" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A263" t="s">
         <v>33</v>
       </c>
@@ -9594,7 +9590,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="264" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="264" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A264" t="s">
         <v>33</v>
       </c>
@@ -9625,7 +9621,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="265" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="265" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A265" t="s">
         <v>33</v>
       </c>
@@ -9656,7 +9652,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="266" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="266" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A266" t="s">
         <v>33</v>
       </c>
@@ -9687,7 +9683,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="267" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="267" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A267" t="s">
         <v>33</v>
       </c>
@@ -9718,7 +9714,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="268" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="268" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A268" t="s">
         <v>33</v>
       </c>
@@ -9749,7 +9745,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="269" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="269" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A269" t="s">
         <v>33</v>
       </c>
@@ -9780,7 +9776,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="270" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="270" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A270" t="s">
         <v>33</v>
       </c>
@@ -9811,7 +9807,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="271" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="271" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A271" t="s">
         <v>33</v>
       </c>
@@ -9842,7 +9838,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="272" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="272" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A272" t="s">
         <v>33</v>
       </c>
@@ -9873,7 +9869,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="273" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="273" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A273" t="s">
         <v>33</v>
       </c>
@@ -9904,7 +9900,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="274" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="274" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A274" t="s">
         <v>33</v>
       </c>
@@ -9935,7 +9931,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="275" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="275" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A275" t="s">
         <v>33</v>
       </c>
@@ -9966,7 +9962,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="276" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="276" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A276" t="s">
         <v>33</v>
       </c>
@@ -9997,7 +9993,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="277" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="277" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A277" t="s">
         <v>33</v>
       </c>
@@ -10028,7 +10024,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="278" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="278" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A278" t="s">
         <v>33</v>
       </c>
@@ -10059,7 +10055,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="279" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="279" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A279" t="s">
         <v>33</v>
       </c>
@@ -10090,7 +10086,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="280" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="280" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A280" t="s">
         <v>33</v>
       </c>
@@ -10121,7 +10117,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="281" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="281" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A281" t="s">
         <v>34</v>
       </c>
@@ -10152,7 +10148,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="282" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="282" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A282" t="s">
         <v>34</v>
       </c>
@@ -10183,7 +10179,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="283" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="283" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A283" t="s">
         <v>34</v>
       </c>
@@ -10214,7 +10210,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="284" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="284" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A284" t="s">
         <v>34</v>
       </c>
@@ -10245,7 +10241,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="285" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="285" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A285" t="s">
         <v>34</v>
       </c>
@@ -10276,7 +10272,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="286" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="286" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A286" t="s">
         <v>34</v>
       </c>
@@ -10307,7 +10303,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="287" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="287" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A287" t="s">
         <v>34</v>
       </c>
@@ -10338,7 +10334,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="288" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="288" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A288" t="s">
         <v>34</v>
       </c>
@@ -10369,7 +10365,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="289" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="289" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A289" t="s">
         <v>34</v>
       </c>
@@ -10400,7 +10396,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="290" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="290" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A290" t="s">
         <v>34</v>
       </c>
@@ -10431,7 +10427,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="291" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="291" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A291" t="s">
         <v>34</v>
       </c>
@@ -10462,7 +10458,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="292" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="292" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A292" t="s">
         <v>34</v>
       </c>
@@ -10493,7 +10489,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="293" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="293" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A293" t="s">
         <v>34</v>
       </c>
@@ -10524,7 +10520,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="294" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="294" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A294" t="s">
         <v>34</v>
       </c>
@@ -10555,7 +10551,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="295" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="295" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A295" t="s">
         <v>34</v>
       </c>
@@ -10586,7 +10582,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="296" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="296" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A296" t="s">
         <v>34</v>
       </c>
@@ -10617,7 +10613,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="297" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="297" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A297" t="s">
         <v>34</v>
       </c>
@@ -10648,7 +10644,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="298" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="298" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A298" t="s">
         <v>34</v>
       </c>
@@ -10679,7 +10675,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="299" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="299" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A299" t="s">
         <v>20</v>
       </c>
@@ -10710,7 +10706,7 @@
         <v>0.23212482221240238</v>
       </c>
     </row>
-    <row r="300" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="300" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A300" t="s">
         <v>20</v>
       </c>
@@ -10741,7 +10737,7 @@
         <v>0.29387295213144909</v>
       </c>
     </row>
-    <row r="301" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="301" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A301" t="s">
         <v>20</v>
       </c>
@@ -10772,7 +10768,7 @@
         <v>0.23644042724023223</v>
       </c>
     </row>
-    <row r="302" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="302" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A302" t="s">
         <v>20</v>
       </c>
@@ -10803,7 +10799,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="303" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="303" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A303" t="s">
         <v>20</v>
       </c>
@@ -10834,7 +10830,7 @@
         <v>0.23644042724023223</v>
       </c>
     </row>
-    <row r="304" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="304" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A304" t="s">
         <v>20</v>
       </c>
@@ -10865,7 +10861,7 @@
         <v>0.29675107064490702</v>
       </c>
     </row>
-    <row r="305" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="305" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A305" t="s">
         <v>20</v>
       </c>
@@ -10896,7 +10892,7 @@
         <v>0.23749502891933028</v>
       </c>
     </row>
-    <row r="306" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="306" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A306" t="s">
         <v>20</v>
       </c>
@@ -10927,7 +10923,7 @@
         <v>0.29745439465101109</v>
       </c>
     </row>
-    <row r="307" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="307" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A307" t="s">
         <v>20</v>
       </c>
@@ -10958,7 +10954,7 @@
         <v>0.23644042724023223</v>
       </c>
     </row>
-    <row r="308" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="308" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A308" t="s">
         <v>20</v>
       </c>
@@ -10989,7 +10985,7 @@
         <v>0.29675107064490702</v>
       </c>
     </row>
-    <row r="309" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="309" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A309" t="s">
         <v>20</v>
       </c>
@@ -11020,7 +11016,7 @@
         <v>0.23537623827314236</v>
       </c>
     </row>
-    <row r="310" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="310" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A310" t="s">
         <v>20</v>
       </c>
@@ -11051,7 +11047,7 @@
         <v>0.29604135278420207</v>
       </c>
     </row>
-    <row r="311" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="311" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A311" t="s">
         <v>20</v>
       </c>
@@ -11082,7 +11078,7 @@
         <v>0.23644042724023223</v>
       </c>
     </row>
-    <row r="312" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="312" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A312" t="s">
         <v>20</v>
       </c>
@@ -11113,7 +11109,7 @@
         <v>0.29675107064490702</v>
       </c>
     </row>
-    <row r="313" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="313" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A313" t="s">
         <v>20</v>
       </c>
@@ -11144,7 +11140,7 @@
         <v>0.23854017228740504</v>
       </c>
     </row>
-    <row r="314" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="314" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A314" t="s">
         <v>20</v>
       </c>
@@ -11175,7 +11171,7 @@
         <v>0.29815141081849533</v>
       </c>
     </row>
-    <row r="315" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="315" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A315" t="s">
         <v>20</v>
       </c>
@@ -11206,7 +11202,7 @@
         <v>0.24060258853373923</v>
       </c>
     </row>
-    <row r="316" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="316" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A316" t="s">
         <v>20</v>
       </c>
@@ -11237,7 +11233,7 @@
         <v>0.29952685605566426</v>
       </c>
     </row>
-    <row r="317" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="317" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A317" t="s">
         <v>33</v>
       </c>
@@ -11268,7 +11264,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="318" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="318" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A318" t="s">
         <v>33</v>
       </c>
@@ -11299,7 +11295,7 @@
         <v>4.537716998313196E-2</v>
       </c>
     </row>
-    <row r="319" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="319" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A319" t="s">
         <v>33</v>
       </c>
@@ -11330,7 +11326,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="320" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="320" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A320" t="s">
         <v>33</v>
       </c>
@@ -11361,7 +11357,7 @@
         <v>4.6178734274645472E-2</v>
       </c>
     </row>
-    <row r="321" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="321" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A321" t="s">
         <v>33</v>
       </c>
@@ -11392,7 +11388,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="322" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="322" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A322" t="s">
         <v>33</v>
       </c>
@@ -11423,7 +11419,7 @@
         <v>5.2372678572595754E-2</v>
       </c>
     </row>
-    <row r="323" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="323" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A323" t="s">
         <v>33</v>
       </c>
@@ -11454,7 +11450,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="324" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="324" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A324" t="s">
         <v>33</v>
       </c>
@@ -11485,7 +11481,7 @@
         <v>4.670480089834822E-2</v>
       </c>
     </row>
-    <row r="325" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="325" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A325" t="s">
         <v>33</v>
       </c>
@@ -11516,7 +11512,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="326" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="326" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A326" t="s">
         <v>33</v>
       </c>
@@ -11547,7 +11543,7 @@
         <v>4.034746970432479E-2</v>
       </c>
     </row>
-    <row r="327" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="327" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A327" t="s">
         <v>33</v>
       </c>
@@ -11578,7 +11574,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="328" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="328" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A328" t="s">
         <v>33</v>
       </c>
@@ -11609,7 +11605,7 @@
         <v>2.464980732392702E-2</v>
       </c>
     </row>
-    <row r="329" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="329" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A329" t="s">
         <v>33</v>
       </c>
@@ -11640,7 +11636,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="330" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="330" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A330" t="s">
         <v>33</v>
       </c>
@@ -11671,7 +11667,7 @@
         <v>2.7511253951581716E-2</v>
       </c>
     </row>
-    <row r="331" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="331" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A331" t="s">
         <v>33</v>
       </c>
@@ -11702,7 +11698,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="332" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="332" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A332" t="s">
         <v>33</v>
       </c>
@@ -11795,7 +11791,7 @@
         <v>6.6234144333528588E-2</v>
       </c>
     </row>
-    <row r="335" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="335" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A335" t="s">
         <v>34</v>
       </c>
@@ -11826,7 +11822,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="336" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="336" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A336" t="s">
         <v>34</v>
       </c>
@@ -11857,7 +11853,7 @@
         <v>5.6490702279729854E-2</v>
       </c>
     </row>
-    <row r="337" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="337" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A337" t="s">
         <v>34</v>
       </c>
@@ -11888,7 +11884,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="338" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="338" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A338" t="s">
         <v>34</v>
       </c>
@@ -11919,7 +11915,7 @@
         <v>5.6490702279729854E-2</v>
       </c>
     </row>
-    <row r="339" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="339" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A339" t="s">
         <v>34</v>
       </c>
@@ -11950,7 +11946,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="340" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="340" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A340" t="s">
         <v>34</v>
       </c>
@@ -11981,7 +11977,7 @@
         <v>5.6490702279729854E-2</v>
       </c>
     </row>
-    <row r="341" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="341" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A341" t="s">
         <v>34</v>
       </c>
@@ -12012,7 +12008,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="342" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="342" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A342" t="s">
         <v>34</v>
       </c>
@@ -12043,7 +12039,7 @@
         <v>5.6490702279729854E-2</v>
       </c>
     </row>
-    <row r="343" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="343" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A343" t="s">
         <v>34</v>
       </c>
@@ -12074,7 +12070,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="344" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="344" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A344" t="s">
         <v>34</v>
       </c>
@@ -12105,7 +12101,7 @@
         <v>5.6490702279729854E-2</v>
       </c>
     </row>
-    <row r="345" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="345" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A345" t="s">
         <v>34</v>
       </c>
@@ -12136,7 +12132,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="346" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="346" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A346" t="s">
         <v>34</v>
       </c>
@@ -12167,7 +12163,7 @@
         <v>5.6490702279729854E-2</v>
       </c>
     </row>
-    <row r="347" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="347" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A347" t="s">
         <v>34</v>
       </c>
@@ -12198,7 +12194,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="348" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="348" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A348" t="s">
         <v>34</v>
       </c>
@@ -12229,7 +12225,7 @@
         <v>5.6490702279729854E-2</v>
       </c>
     </row>
-    <row r="349" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="349" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A349" t="s">
         <v>34</v>
       </c>
@@ -12260,7 +12256,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="350" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="350" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A350" t="s">
         <v>34</v>
       </c>
@@ -12291,7 +12287,7 @@
         <v>5.6490702279729854E-2</v>
       </c>
     </row>
-    <row r="351" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="351" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A351" t="s">
         <v>34</v>
       </c>
@@ -12322,7 +12318,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="352" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="352" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A352" t="s">
         <v>34</v>
       </c>
@@ -12353,7 +12349,7 @@
         <v>5.6490702279729854E-2</v>
       </c>
     </row>
-    <row r="353" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="353" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A353" t="s">
         <v>20</v>
       </c>
@@ -12384,7 +12380,7 @@
         <v>0.28355244879404107</v>
       </c>
     </row>
-    <row r="354" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="354" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A354" t="s">
         <v>20</v>
       </c>
@@ -12415,7 +12411,7 @@
         <v>0.34041129914404022</v>
       </c>
     </row>
-    <row r="355" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="355" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A355" t="s">
         <v>20</v>
       </c>
@@ -12446,7 +12442,7 @@
         <v>0.28693723705116253</v>
       </c>
     </row>
-    <row r="356" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="356" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A356" t="s">
         <v>20</v>
       </c>
@@ -12477,7 +12473,7 @@
         <v>0.34244709463464579</v>
       </c>
     </row>
-    <row r="357" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="357" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A357" t="s">
         <v>20</v>
       </c>
@@ -12508,7 +12504,7 @@
         <v>0.28693723705116253</v>
       </c>
     </row>
-    <row r="358" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="358" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A358" t="s">
         <v>20</v>
       </c>
@@ -12539,7 +12535,7 @@
         <v>0.34244709463464579</v>
       </c>
     </row>
-    <row r="359" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="359" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A359" t="s">
         <v>20</v>
       </c>
@@ -12570,7 +12566,7 @@
         <v>0.28776437562300416</v>
       </c>
     </row>
-    <row r="360" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="360" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A360" t="s">
         <v>20</v>
       </c>
@@ -12601,7 +12597,7 @@
         <v>0.34294458069485012</v>
       </c>
     </row>
-    <row r="361" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="361" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A361" t="s">
         <v>20</v>
       </c>
@@ -12632,7 +12628,7 @@
         <v>0.28693723705116253</v>
       </c>
     </row>
-    <row r="362" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="362" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A362" t="s">
         <v>20</v>
       </c>
@@ -12663,7 +12659,7 @@
         <v>0.34244709463464579</v>
       </c>
     </row>
-    <row r="363" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="363" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A363" t="s">
         <v>20</v>
       </c>
@@ -12694,7 +12690,7 @@
         <v>0.28610257903775871</v>
       </c>
     </row>
-    <row r="364" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="364" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A364" t="s">
         <v>20</v>
       </c>
@@ -12725,7 +12721,7 @@
         <v>0.34194508597389417</v>
       </c>
     </row>
-    <row r="365" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="365" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A365" t="s">
         <v>20</v>
       </c>
@@ -12756,7 +12752,7 @@
         <v>0.28693723705116253</v>
       </c>
     </row>
-    <row r="366" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="366" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A366" t="s">
         <v>20</v>
       </c>
@@ -12787,7 +12783,7 @@
         <v>0.34244709463464579</v>
       </c>
     </row>
-    <row r="367" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="367" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A367" t="s">
         <v>20</v>
       </c>
@@ -12818,7 +12814,7 @@
         <v>0.28858409591169021</v>
       </c>
     </row>
-    <row r="368" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="368" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A368" t="s">
         <v>20</v>
       </c>
@@ -12849,7 +12845,7 @@
         <v>0.34343760499666692</v>
       </c>
     </row>
-    <row r="369" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="369" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A369" t="s">
         <v>20</v>
       </c>
@@ -12880,7 +12876,7 @@
         <v>0.29020167728136409</v>
       </c>
     </row>
-    <row r="370" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="370" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A370" t="s">
         <v>20</v>
       </c>
@@ -12911,7 +12907,7 @@
         <v>0.34441050628558545</v>
       </c>
     </row>
-    <row r="371" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="371" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A371" t="s">
         <v>33</v>
       </c>
@@ -12942,7 +12938,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="372" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="372" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A372" t="s">
         <v>33</v>
       </c>
@@ -12973,7 +12969,7 @@
         <v>0.16464140281539436</v>
       </c>
     </row>
-    <row r="373" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="373" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A373" t="s">
         <v>33</v>
       </c>
@@ -13004,7 +13000,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="374" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="374" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A374" t="s">
         <v>33</v>
       </c>
@@ -13035,7 +13031,7 @@
         <v>0.1652083777201675</v>
       </c>
     </row>
-    <row r="375" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="375" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A375" t="s">
         <v>33</v>
       </c>
@@ -13066,7 +13062,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="376" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="376" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A376" t="s">
         <v>33</v>
       </c>
@@ -13097,7 +13093,7 @@
         <v>0.16958957460690705</v>
       </c>
     </row>
-    <row r="377" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="377" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A377" t="s">
         <v>33</v>
       </c>
@@ -13128,7 +13124,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="378" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="378" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A378" t="s">
         <v>33</v>
       </c>
@@ -13159,7 +13155,7 @@
         <v>0.16558048333544517</v>
       </c>
     </row>
-    <row r="379" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="379" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A379" t="s">
         <v>33</v>
       </c>
@@ -13190,7 +13186,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="380" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="380" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A380" t="s">
         <v>33</v>
       </c>
@@ -13221,7 +13217,7 @@
         <v>0.1610837170916084</v>
       </c>
     </row>
-    <row r="381" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="381" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A381" t="s">
         <v>33</v>
       </c>
@@ -13252,7 +13248,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="382" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="382" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A382" t="s">
         <v>33</v>
       </c>
@@ -13283,7 +13279,7 @@
         <v>0.14998020271663298</v>
       </c>
     </row>
-    <row r="383" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="383" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A383" t="s">
         <v>33</v>
       </c>
@@ -13314,7 +13310,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="384" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="384" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A384" t="s">
         <v>33</v>
       </c>
@@ -13345,7 +13341,7 @@
         <v>0.15200420559002026</v>
       </c>
     </row>
-    <row r="385" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="385" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A385" t="s">
         <v>33</v>
       </c>
@@ -13376,7 +13372,7 @@
         <v>2.3087042915230227E-3</v>
       </c>
     </row>
-    <row r="386" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="386" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A386" t="s">
         <v>33</v>
       </c>
@@ -13407,7 +13403,7 @@
         <v>0.17125603644344589</v>
       </c>
     </row>
-    <row r="387" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="387" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A387" t="s">
         <v>33</v>
       </c>
@@ -13438,7 +13434,7 @@
         <v>1.5839649652288679E-2</v>
       </c>
     </row>
-    <row r="388" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="388" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A388" t="s">
         <v>33</v>
       </c>
@@ -13469,7 +13465,7 @@
         <v>0.17939428186873113</v>
       </c>
     </row>
-    <row r="389" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="389" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A389" t="s">
         <v>34</v>
       </c>
@@ -13500,7 +13496,7 @@
         <v>4.3809525578395458E-3</v>
       </c>
     </row>
-    <row r="390" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="390" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A390" t="s">
         <v>34</v>
       </c>
@@ -13531,7 +13527,7 @@
         <v>0.17250239909762566</v>
       </c>
     </row>
-    <row r="391" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="391" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A391" t="s">
         <v>34</v>
       </c>
@@ -13562,7 +13558,7 @@
         <v>4.3809525578395458E-3</v>
       </c>
     </row>
-    <row r="392" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="392" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A392" t="s">
         <v>34</v>
       </c>
@@ -13593,7 +13589,7 @@
         <v>0.17250239909762566</v>
       </c>
     </row>
-    <row r="393" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="393" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A393" t="s">
         <v>34</v>
       </c>
@@ -13624,7 +13620,7 @@
         <v>4.3809525578395458E-3</v>
       </c>
     </row>
-    <row r="394" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="394" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A394" t="s">
         <v>34</v>
       </c>
@@ -13655,7 +13651,7 @@
         <v>0.17250239909762566</v>
       </c>
     </row>
-    <row r="395" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="395" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A395" t="s">
         <v>34</v>
       </c>
@@ -13686,7 +13682,7 @@
         <v>4.3809525578395458E-3</v>
       </c>
     </row>
-    <row r="396" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="396" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A396" t="s">
         <v>34</v>
       </c>
@@ -13717,7 +13713,7 @@
         <v>0.17250239909762566</v>
       </c>
     </row>
-    <row r="397" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="397" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A397" t="s">
         <v>34</v>
       </c>
@@ -13748,7 +13744,7 @@
         <v>4.3809525578395458E-3</v>
       </c>
     </row>
-    <row r="398" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="398" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A398" t="s">
         <v>34</v>
       </c>
@@ -13779,7 +13775,7 @@
         <v>0.17250239909762566</v>
       </c>
     </row>
-    <row r="399" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="399" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A399" t="s">
         <v>34</v>
       </c>
@@ -13810,7 +13806,7 @@
         <v>4.3809525578395458E-3</v>
       </c>
     </row>
-    <row r="400" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="400" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A400" t="s">
         <v>34</v>
       </c>
@@ -13841,7 +13837,7 @@
         <v>0.17250239909762566</v>
       </c>
     </row>
-    <row r="401" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="401" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A401" t="s">
         <v>34</v>
       </c>
@@ -13872,7 +13868,7 @@
         <v>4.3809525578395458E-3</v>
       </c>
     </row>
-    <row r="402" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="402" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A402" t="s">
         <v>34</v>
       </c>
@@ -13903,7 +13899,7 @@
         <v>0.17250239909762566</v>
       </c>
     </row>
-    <row r="403" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="403" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A403" t="s">
         <v>34</v>
       </c>
@@ -13934,7 +13930,7 @@
         <v>4.3809525578395458E-3</v>
       </c>
     </row>
-    <row r="404" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="404" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A404" t="s">
         <v>34</v>
       </c>
@@ -13965,7 +13961,7 @@
         <v>0.17250239909762566</v>
       </c>
     </row>
-    <row r="405" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="405" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A405" t="s">
         <v>34</v>
       </c>
@@ -13996,7 +13992,7 @@
         <v>4.3809525578395458E-3</v>
       </c>
     </row>
-    <row r="406" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="406" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A406" t="s">
         <v>34</v>
       </c>
@@ -14027,7 +14023,7 @@
         <v>0.17250239909762566</v>
       </c>
     </row>
-    <row r="407" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="407" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A407" t="s">
         <v>46</v>
       </c>
@@ -14060,7 +14056,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="408" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="408" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A408" t="s">
         <v>46</v>
       </c>
@@ -14093,7 +14089,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="409" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="409" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A409" t="s">
         <v>46</v>
       </c>
@@ -14127,7 +14123,13 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:M1" xr:uid="{97D578EE-3C05-4D0C-AE17-43AAD0A9E4AC}"/>
+  <autoFilter ref="A1:M409" xr:uid="{97D578EE-3C05-4D0C-AE17-43AAD0A9E4AC}">
+    <filterColumn colId="3">
+      <filters>
+        <filter val="IEA - 2019 - Average"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -14137,13 +14139,10 @@
   <sheetPr>
     <tabColor rgb="FF00B0F0"/>
   </sheetPr>
-  <dimension ref="A1:E26"/>
+  <dimension ref="A1:E29"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A17" sqref="A17"/>
-    </sheetView>
-    <sheetView tabSelected="1" workbookViewId="1">
-      <selection activeCell="M13" sqref="M13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -14420,6 +14419,12 @@
       </c>
       <c r="D26" t="s">
         <v>19</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C29">
+        <f>C12*C22*Prices!D71</f>
+        <v>0.35697451493784776</v>
       </c>
     </row>
   </sheetData>
@@ -14436,7 +14441,6 @@
   <dimension ref="A1:N109"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
-    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -16098,7 +16102,6 @@
   <dimension ref="A1:J6"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
-    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -16282,7 +16285,6 @@
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
-    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -16340,10 +16342,7 @@
   </sheetPr>
   <dimension ref="A1:J5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:XFD3"/>
-    </sheetView>
-    <sheetView workbookViewId="1"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -16519,10 +16518,7 @@
   </sheetPr>
   <dimension ref="A1:J5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3:J3"/>
-    </sheetView>
-    <sheetView workbookViewId="1"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -16702,10 +16698,7 @@
   </sheetPr>
   <dimension ref="A1:J5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:J5"/>
-    </sheetView>
-    <sheetView workbookViewId="1"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>

</xml_diff>

<commit_message>
added assumptions on capacity factors in plot titles
</commit_message>
<xml_diff>
--- a/Shocks/ShockMaster.xlsx
+++ b/Shocks/ShockMaster.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\loren\Documents\GitHub\MARIO Organization\GreenTechs\Shocks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4D7FCE8-9A4C-4365-90C1-D78328CECECF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E802770-CD1E-4BD4-A646-E463DFB4934D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="39852" yWindow="0" windowWidth="9396" windowHeight="13200" activeTab="1" xr2:uid="{B60DDE52-988F-44A2-B15C-F9EEC5148EBF}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{B60DDE52-988F-44A2-B15C-F9EEC5148EBF}"/>
   </bookViews>
   <sheets>
     <sheet name="ShockMaster" sheetId="6" r:id="rId1"/>
@@ -14142,7 +14142,7 @@
   <dimension ref="A1:E29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="K8" sqref="K8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>